<commit_message>
Changed the system to add alloy sorting
</commit_message>
<xml_diff>
--- a/data/ODYM_Classifications_Master_Al_cars.xlsx
+++ b/data/ODYM_Classifications_Master_Al_cars.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\model with segments and powertrain\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9D616C-EEB4-4BF7-8B80-F7810AF6CAAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF3D06D-AA1B-4FF6-8B86-183D0E537589}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="10" xr2:uid="{DB6AE323-0020-4BE8-9888-EBD3E10A18BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="3" activeTab="10" xr2:uid="{DB6AE323-0020-4BE8-9888-EBD3E10A18BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover_Dimensions_Aspects" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="MAIN_Table" sheetId="2" r:id="rId11"/>
     <sheet name="Scenario" sheetId="11" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateCount="1000"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="336">
   <si>
     <t>ODYM Classifications master file, tutorial version</t>
   </si>
@@ -1050,6 +1050,9 @@
   <si>
     <t>Aluminum Alloys</t>
   </si>
+  <si>
+    <t>Aluminium</t>
+  </si>
 </sst>
 </file>
 
@@ -1774,8 +1777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E68962F-C18C-465A-8142-6DB1BD1DEB4A}">
   <dimension ref="A1:L1311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2260,9 +2263,8 @@
         <f>Powertrain!D2</f>
         <v>ICEV</v>
       </c>
-      <c r="H11" t="str">
-        <f>Goods!D2</f>
-        <v>Food</v>
+      <c r="H11" t="s">
+        <v>335</v>
       </c>
       <c r="I11" t="str">
         <f>Segment!D2</f>
@@ -39326,7 +39328,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Adding lifetime and alloy sorrting scenarios to parameters
</commit_message>
<xml_diff>
--- a/data/ODYM_Classifications_Master_Al_cars.xlsx
+++ b/data/ODYM_Classifications_Master_Al_cars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6189F4-3F4A-421F-9798-BB708CAAD752}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C301EA-CB9F-4E0E-A43F-FD84880E2F50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-315" windowWidth="38640" windowHeight="21240" firstSheet="7" activeTab="16" xr2:uid="{DB6AE323-0020-4BE8-9888-EBD3E10A18BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="10" activeTab="18" xr2:uid="{DB6AE323-0020-4BE8-9888-EBD3E10A18BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover_Dimensions_Aspects" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,10 @@
     <sheet name="Powertrain_Scenario" sheetId="18" r:id="rId13"/>
     <sheet name="Segment_Scenario" sheetId="19" r:id="rId14"/>
     <sheet name="Al_Content_Scenario" sheetId="17" r:id="rId15"/>
-    <sheet name="Carbon_Footprint_Scenario" sheetId="11" r:id="rId16"/>
-    <sheet name="MAIN_Table" sheetId="2" r:id="rId17"/>
+    <sheet name="Lifetime_Scenario" sheetId="20" r:id="rId16"/>
+    <sheet name="Alloy_Sorting_Scenario" sheetId="21" r:id="rId17"/>
+    <sheet name="Carbon_Footprint_Scenario" sheetId="11" r:id="rId18"/>
+    <sheet name="MAIN_Table" sheetId="2" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="357">
   <si>
     <t>ODYM Classifications master file, tutorial version</t>
   </si>
@@ -268,9 +270,6 @@
   </si>
   <si>
     <t>Scenario</t>
-  </si>
-  <si>
-    <t>945a49ba-8ee6-4d97-ac63-0da6eb207e7a</t>
   </si>
   <si>
     <t>Baseline</t>
@@ -1112,6 +1111,18 @@
   <si>
     <t>Scenarios for carbon footprint of Al production</t>
   </si>
+  <si>
+    <t>Lifetime_Scenario</t>
+  </si>
+  <si>
+    <t>Scenarios for average lifetime of cars</t>
+  </si>
+  <si>
+    <t>Alloy_Sorting_Scenario</t>
+  </si>
+  <si>
+    <t>Scenarios for alloy sorting technology penetration</t>
+  </si>
 </sst>
 </file>
 
@@ -1714,10 +1725,10 @@
         <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -1747,7 +1758,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -1778,7 +1789,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D3" t="s">
         <v>70</v>
@@ -1866,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -1886,7 +1897,7 @@
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1899,10 +1910,10 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1918,7 +1929,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1958,7 +1969,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F8" s="2"/>
       <c r="H8" s="2"/>
@@ -2007,7 +2018,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -2027,7 +2038,7 @@
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2040,10 +2051,10 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2059,7 +2070,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2099,7 +2110,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F8" s="2"/>
       <c r="H8" s="2"/>
@@ -2148,7 +2159,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -2168,7 +2179,7 @@
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2181,10 +2192,10 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2200,7 +2211,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2213,7 +2224,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -2246,7 +2257,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F8" s="2"/>
       <c r="H8" s="2"/>
@@ -2295,7 +2306,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -2315,7 +2326,7 @@
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2328,10 +2339,10 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2347,7 +2358,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2360,7 +2371,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -2393,7 +2404,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F8" s="2"/>
       <c r="H8" s="2"/>
@@ -2426,7 +2437,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D2" sqref="D2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2442,7 +2453,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -2462,7 +2473,7 @@
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2475,10 +2486,10 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2494,7 +2505,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2534,7 +2545,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F8" s="2"/>
       <c r="H8" s="2"/>
@@ -2563,11 +2574,11 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B125EA6-3B3A-4833-AC82-0D4BFE55E786}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6C9230-52FA-44B8-B152-D0E0E7BC59B5}">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+      <selection activeCell="D2" sqref="D2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2583,7 +2594,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -2603,7 +2614,7 @@
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2616,10 +2627,10 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2635,7 +2646,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2647,9 +2658,6 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
-        <v>73</v>
-      </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -2657,7 +2665,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="6">
-        <v>43979</v>
+        <v>44312</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -2666,7 +2674,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="6">
-        <v>44005</v>
+        <v>44312</v>
       </c>
       <c r="F7" s="2"/>
       <c r="H7" s="2"/>
@@ -2676,7 +2684,289 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="F9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FDE2DD4-51F6-4111-9141-4DC3E0FDBB3A}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>356</v>
+      </c>
+      <c r="D3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>335</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="6">
+        <v>44312</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6">
+        <v>44312</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="F9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B125EA6-3B3A-4833-AC82-0D4BFE55E786}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>351</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="6">
+        <v>44312</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6">
+        <v>44312</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
       </c>
       <c r="F8" s="2"/>
       <c r="H8" s="2"/>
@@ -2707,12 +2997,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E68962F-C18C-465A-8142-6DB1BD1DEB4A}">
-  <dimension ref="A1:Q1311"/>
+  <dimension ref="A1:S1311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14:Q21"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2730,9 +3020,11 @@
     <col min="12" max="13" width="37.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="37.5546875" customWidth="1"/>
     <col min="15" max="17" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="41.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2796,11 +3088,19 @@
         <v>Al_Content_Scenario</v>
       </c>
       <c r="Q1" s="1" t="str">
+        <f>Lifetime_Scenario!B1</f>
+        <v>Lifetime_Scenario</v>
+      </c>
+      <c r="R1" s="1" t="str">
+        <f>Alloy_Sorting_Scenario!B1</f>
+        <v>Alloy_Sorting_Scenario</v>
+      </c>
+      <c r="S1" s="1" t="str">
         <f>Carbon_Footprint_Scenario!B1</f>
         <v>Carbon_Footprint_Scenario</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -2864,11 +3164,19 @@
         <v>Scenario</v>
       </c>
       <c r="Q2" t="str">
+        <f>Lifetime_Scenario!B2</f>
+        <v>Scenario</v>
+      </c>
+      <c r="R2" t="str">
+        <f>Alloy_Sorting_Scenario!B2</f>
+        <v>Scenario</v>
+      </c>
+      <c r="S2" t="str">
         <f>Carbon_Footprint_Scenario!B2</f>
         <v>Scenario</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -2932,11 +3240,19 @@
         <v>Scenarios for average Al content</v>
       </c>
       <c r="Q3" t="str">
+        <f>Lifetime_Scenario!B3</f>
+        <v>Scenarios for average lifetime of cars</v>
+      </c>
+      <c r="R3" t="str">
+        <f>Alloy_Sorting_Scenario!B3</f>
+        <v>Scenarios for alloy sorting technology penetration</v>
+      </c>
+      <c r="S3" t="str">
         <f>Carbon_Footprint_Scenario!B3</f>
         <v>Scenarios for carbon footprint of Al production</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -3000,11 +3316,19 @@
         <v>None</v>
       </c>
       <c r="Q4" t="str">
+        <f>Lifetime_Scenario!B4</f>
+        <v>None</v>
+      </c>
+      <c r="R4" t="str">
+        <f>Alloy_Sorting_Scenario!B4</f>
+        <v>None</v>
+      </c>
+      <c r="S4" t="str">
         <f>Carbon_Footprint_Scenario!B4</f>
         <v>None</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -3064,12 +3388,20 @@
         <f>Al_Content_Scenario!B5</f>
         <v>0</v>
       </c>
-      <c r="Q5" t="str">
+      <c r="Q5">
+        <f>Lifetime_Scenario!B5</f>
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <f>Alloy_Sorting_Scenario!B5</f>
+        <v>0</v>
+      </c>
+      <c r="S5">
         <f>Carbon_Footprint_Scenario!B5</f>
-        <v>945a49ba-8ee6-4d97-ac63-0da6eb207e7a</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -3133,11 +3465,19 @@
         <v>44295</v>
       </c>
       <c r="Q6" s="14">
+        <f>Lifetime_Scenario!B6</f>
+        <v>44312</v>
+      </c>
+      <c r="R6" s="14">
+        <f>Alloy_Sorting_Scenario!B6</f>
+        <v>44312</v>
+      </c>
+      <c r="S6" s="14">
         <f>Carbon_Footprint_Scenario!B6</f>
-        <v>43979</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+        <v>44312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -3201,11 +3541,19 @@
         <v>44295</v>
       </c>
       <c r="Q7" s="15">
+        <f>Lifetime_Scenario!B7</f>
+        <v>44312</v>
+      </c>
+      <c r="R7" s="15">
+        <f>Alloy_Sorting_Scenario!B7</f>
+        <v>44312</v>
+      </c>
+      <c r="S7" s="15">
         <f>Carbon_Footprint_Scenario!B7</f>
-        <v>44005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+        <v>44312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -3267,11 +3615,19 @@
         <v>Romain Billy</v>
       </c>
       <c r="Q8" s="9" t="str">
+        <f>Lifetime_Scenario!B8</f>
+        <v>Romain Billy</v>
+      </c>
+      <c r="R8" s="9" t="str">
+        <f>Alloy_Sorting_Scenario!B8</f>
+        <v>Romain Billy</v>
+      </c>
+      <c r="S8" s="9" t="str">
         <f>Carbon_Footprint_Scenario!B8</f>
         <v>Romain Billy</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -3333,11 +3689,19 @@
         <v>0</v>
       </c>
       <c r="Q9" s="9">
+        <f>Lifetime_Scenario!B9</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="9">
+        <f>Alloy_Sorting_Scenario!B9</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="9">
         <f>Carbon_Footprint_Scenario!B9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>26</v>
       </c>
@@ -3356,8 +3720,10 @@
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -3385,7 +3751,7 @@
         <v>ICEV</v>
       </c>
       <c r="H11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I11" t="str">
         <f>Segment!D2</f>
@@ -3420,11 +3786,19 @@
         <v>Low</v>
       </c>
       <c r="Q11" t="str">
+        <f>Lifetime_Scenario!D2</f>
+        <v>Low</v>
+      </c>
+      <c r="R11" t="str">
+        <f>Alloy_Sorting_Scenario!D2</f>
+        <v>Low</v>
+      </c>
+      <c r="S11" t="str">
         <f>Carbon_Footprint_Scenario!D2</f>
         <v>Constant</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -3481,11 +3855,19 @@
         <v>Medium</v>
       </c>
       <c r="Q12" t="str">
+        <f>Lifetime_Scenario!D3</f>
+        <v>Medium</v>
+      </c>
+      <c r="R12" t="str">
+        <f>Alloy_Sorting_Scenario!D3</f>
+        <v>Medium</v>
+      </c>
+      <c r="S12" t="str">
         <f>Carbon_Footprint_Scenario!D3</f>
         <v>Medium</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -3542,11 +3924,19 @@
         <v>High</v>
       </c>
       <c r="Q13" t="str">
+        <f>Lifetime_Scenario!D4</f>
+        <v>High</v>
+      </c>
+      <c r="R13" t="str">
+        <f>Alloy_Sorting_Scenario!D4</f>
+        <v>High</v>
+      </c>
+      <c r="S13" t="str">
         <f>Carbon_Footprint_Scenario!D4</f>
         <v>IAI_B2DS</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>3</v>
       </c>
@@ -3587,7 +3977,7 @@
         <v>Constant</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -3612,7 +4002,7 @@
         <v>G5</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>5</v>
       </c>
@@ -17550,7 +17940,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8">
         <v>1706</v>
@@ -27944,7 +28334,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
@@ -27976,7 +28366,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D3">
         <v>1701</v>
@@ -28043,7 +28433,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8">
         <v>1706</v>
@@ -38457,13 +38847,13 @@
         <v>39</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -38471,16 +38861,16 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>77</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>78</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -38491,13 +38881,13 @@
         <v>28</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -38508,13 +38898,13 @@
         <v>40</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -38525,13 +38915,13 @@
         <v>43028</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -38542,13 +38932,13 @@
         <v>43028</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -38556,7 +38946,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>53</v>
@@ -38565,7 +38955,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -38574,68 +38964,68 @@
       </c>
       <c r="B9" s="16"/>
       <c r="D9" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9">
         <v>7</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D10" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E10">
         <v>8</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E11">
         <v>9</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E13">
         <v>11</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E14">
         <v>12</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -38646,711 +39036,711 @@
         <v>13</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E16">
         <v>14</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D17" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E17">
         <v>15</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D18" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E18">
         <v>16</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D19" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E19">
         <v>17</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D20" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E20">
         <v>18</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D21" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E21">
         <v>19</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D22" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E22">
         <v>20</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D23" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E23">
         <v>21</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D24" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E24">
         <v>22</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D25" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E25">
         <v>23</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D26" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E26">
         <v>24</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D27" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E27">
         <v>25</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D28" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E28">
         <v>26</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D29" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E29">
         <v>27</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D30" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E30">
         <v>28</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D31" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E31">
         <v>29</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D32" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E32">
         <v>30</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D33" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E33">
         <v>31</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D34" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E34">
         <v>32</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D35" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E35">
         <v>33</v>
       </c>
       <c r="F35" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D36" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E36">
         <v>34</v>
       </c>
       <c r="F36" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D37" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E37">
         <v>35</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D38" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E38">
         <v>36</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D39" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E39">
         <v>37</v>
       </c>
       <c r="F39" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D40" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E40">
         <v>38</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D41" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E41">
         <v>39</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D42" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E42">
         <v>40</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D43" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E43">
         <v>41</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D44" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E44">
         <v>42</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D45" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E45">
         <v>43</v>
       </c>
       <c r="F45" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D46" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E46">
         <v>44</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D47" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E47">
         <v>45</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D48" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E48">
         <v>46</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D49" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E49">
         <v>47</v>
       </c>
       <c r="F49" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D50" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E50">
         <v>48</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D51" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E51">
         <v>49</v>
       </c>
       <c r="F51" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D52" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E52">
         <v>50</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D53" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E53">
         <v>51</v>
       </c>
       <c r="F53" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D54" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E54">
         <v>52</v>
       </c>
       <c r="F54" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D55" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E55">
         <v>53</v>
       </c>
       <c r="F55" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D56" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E56">
         <v>54</v>
       </c>
       <c r="F56" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="57" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D57" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E57">
         <v>55</v>
       </c>
       <c r="F57" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="58" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D58" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E58">
         <v>56</v>
       </c>
       <c r="F58" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="59" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D59" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E59">
         <v>57</v>
       </c>
       <c r="F59" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D60" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E60">
         <v>58</v>
       </c>
       <c r="F60" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="61" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D61" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E61">
         <v>59</v>
       </c>
       <c r="F61" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="62" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D62" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E62">
         <v>60</v>
       </c>
       <c r="F62" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="63" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D63" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E63">
         <v>61</v>
       </c>
       <c r="F63" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D64" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E64">
         <v>62</v>
       </c>
       <c r="F64" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D65" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E65">
         <v>63</v>
       </c>
       <c r="F65" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D66" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E66">
         <v>64</v>
       </c>
       <c r="F66" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D67" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E67">
         <v>65</v>
       </c>
       <c r="F67" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D68" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E68">
         <v>66</v>
       </c>
       <c r="F68" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D69" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E69">
         <v>67</v>
       </c>
       <c r="F69" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="70" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D70" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E70">
         <v>68</v>
       </c>
       <c r="F70" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D71" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E71">
         <v>69</v>
       </c>
       <c r="F71" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="72" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D72" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E72">
         <v>70</v>
       </c>
       <c r="F72" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D73" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E73">
         <v>71</v>
       </c>
       <c r="F73" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="74" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D74" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E74">
         <v>72</v>
       </c>
       <c r="F74" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="75" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D75" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E75">
         <v>73</v>
       </c>
       <c r="F75" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="76" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D76" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E76">
         <v>74</v>
       </c>
       <c r="F76" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="77" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D77" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E77">
         <v>75</v>
       </c>
       <c r="F77" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="78" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D78" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E78">
         <v>76</v>
       </c>
       <c r="F78" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="79" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D79" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E79">
         <v>77</v>
       </c>
       <c r="F79" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="80" spans="4:6" x14ac:dyDescent="0.3">
@@ -39361,249 +39751,249 @@
         <v>78</v>
       </c>
       <c r="F80" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="81" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D81" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E81">
         <v>79</v>
       </c>
       <c r="F81" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="82" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D82" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E82">
         <v>80</v>
       </c>
       <c r="F82" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="83" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D83" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E83">
         <v>81</v>
       </c>
       <c r="F83" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="84" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D84" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E84">
         <v>82</v>
       </c>
       <c r="F84" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="85" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D85" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E85">
         <v>83</v>
       </c>
       <c r="F85" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="86" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D86" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E86">
         <v>84</v>
       </c>
       <c r="F86" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="87" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D87" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E87">
         <v>85</v>
       </c>
       <c r="F87" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D88" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E88">
         <v>86</v>
       </c>
       <c r="F88" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="89" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D89" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E89">
         <v>87</v>
       </c>
       <c r="F89" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D90" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E90">
         <v>88</v>
       </c>
       <c r="F90" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="91" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D91" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E91">
         <v>89</v>
       </c>
       <c r="F91" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="92" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D92" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E92">
         <v>90</v>
       </c>
       <c r="F92" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="93" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D93" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E93">
         <v>91</v>
       </c>
       <c r="F93" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="94" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D94" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E94">
         <v>92</v>
       </c>
       <c r="F94" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="95" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D95" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E95">
         <v>93</v>
       </c>
       <c r="F95" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="96" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D96" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E96">
         <v>94</v>
       </c>
       <c r="F96" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="97" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D97" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E97">
         <v>95</v>
       </c>
       <c r="F97" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="98" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D98" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E98">
         <v>96</v>
       </c>
       <c r="F98" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="99" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D99" s="18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E99">
         <v>97</v>
       </c>
       <c r="F99" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="100" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D100" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E100">
         <v>98</v>
       </c>
       <c r="F100" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="101" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D101" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E101">
         <v>99</v>
       </c>
       <c r="F101" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="102" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D102" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E102">
         <v>100</v>
       </c>
       <c r="F102" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -39634,7 +40024,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -39654,7 +40044,7 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -39665,7 +40055,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D3" t="s">
         <v>53</v>
@@ -39682,7 +40072,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -39693,10 +40083,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>313</v>
+      </c>
+      <c r="D5" t="s">
         <v>314</v>
-      </c>
-      <c r="D5" t="s">
-        <v>315</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -39896,10 +40286,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -39920,7 +40310,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -39932,10 +40322,10 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" t="s">
         <v>277</v>
-      </c>
-      <c r="D3" t="s">
-        <v>278</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -39950,14 +40340,14 @@
         <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -39965,16 +40355,16 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>280</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>282</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -39985,13 +40375,13 @@
         <v>43028</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -40002,7 +40392,7 @@
         <v>43058</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -40013,10 +40403,10 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -40028,7 +40418,7 @@
       </c>
       <c r="B9" s="16"/>
       <c r="D9" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -40037,7 +40427,7 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="D10" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -40054,7 +40444,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E12">
         <v>10</v>
@@ -40062,7 +40452,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D13" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E13">
         <v>11</v>
@@ -40070,7 +40460,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E14">
         <v>12</v>
@@ -40078,7 +40468,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D15" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E15">
         <v>13</v>
@@ -40086,7 +40476,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D16" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E16">
         <v>14</v>
@@ -40094,18 +40484,18 @@
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D17" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E17">
         <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D18" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -40113,7 +40503,7 @@
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D19" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E19">
         <v>17</v>
@@ -40121,7 +40511,7 @@
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D20" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E20">
         <v>18</v>
@@ -40129,7 +40519,7 @@
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D21" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E21">
         <v>19</v>
@@ -40137,7 +40527,7 @@
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D22" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E22">
         <v>20</v>
@@ -40145,7 +40535,7 @@
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D23" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E23">
         <v>21</v>
@@ -40153,7 +40543,7 @@
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D24" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E24">
         <v>22</v>
@@ -40161,7 +40551,7 @@
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D25" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E25">
         <v>23</v>
@@ -40169,7 +40559,7 @@
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D26" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E26">
         <v>24</v>
@@ -40177,7 +40567,7 @@
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D27" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E27">
         <v>25</v>
@@ -40185,7 +40575,7 @@
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D28" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E28">
         <v>26</v>
@@ -40193,7 +40583,7 @@
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D29" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E29">
         <v>27</v>
@@ -40201,7 +40591,7 @@
     </row>
     <row r="30" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D30" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E30">
         <v>28</v>
@@ -40209,7 +40599,7 @@
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D31" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E31">
         <v>29</v>
@@ -40217,7 +40607,7 @@
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D32" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E32">
         <v>30</v>
@@ -40251,7 +40641,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -40271,7 +40661,7 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -40282,10 +40672,10 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3" t="s">
         <v>317</v>
-      </c>
-      <c r="D3" t="s">
-        <v>318</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -40299,7 +40689,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -40310,10 +40700,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>319</v>
+      </c>
+      <c r="D5" t="s">
         <v>320</v>
-      </c>
-      <c r="D5" t="s">
-        <v>321</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -40376,7 +40766,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Updated values for NZE
updated values for NZE scenarios and clean some data and result files after merging
</commit_message>
<xml_diff>
--- a/data/ODYM_Classifications_Master_Al_cars.xlsx
+++ b/data/ODYM_Classifications_Master_Al_cars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03527AF-3929-416E-8A56-B824F347074B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5808B0A4-7DAD-4635-A723-4DB53296FC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="10" activeTab="18" xr2:uid="{DB6AE323-0020-4BE8-9888-EBD3E10A18BE}"/>
+    <workbookView xWindow="-38520" yWindow="90" windowWidth="38640" windowHeight="21240" firstSheet="10" activeTab="18" xr2:uid="{DB6AE323-0020-4BE8-9888-EBD3E10A18BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover_Dimensions_Aspects" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="358">
   <si>
     <t>ODYM Classifications master file, tutorial version</t>
   </si>
@@ -1123,6 +1123,9 @@
   <si>
     <t>Scenarios for alloy sorting technology penetration</t>
   </si>
+  <si>
+    <t>NZE</t>
+  </si>
 </sst>
 </file>
 
@@ -3002,7 +3005,7 @@
   <dimension ref="A1:S1311"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3912,8 +3915,8 @@
         <v>High</v>
       </c>
       <c r="N13" t="str">
-        <f>Powertrain_Scenario!D4</f>
-        <v>High_EV</v>
+        <f>Powertrain_Scenario!D5</f>
+        <v>Constant</v>
       </c>
       <c r="O13" t="str">
         <f>Segment_Scenario!D4</f>
@@ -3968,9 +3971,8 @@
         <f>Component!D5</f>
         <v>G4</v>
       </c>
-      <c r="N14" t="str">
-        <f>Powertrain_Scenario!D5</f>
-        <v>Constant</v>
+      <c r="N14" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>